<commit_message>
Functional Simulation of Bus Routes
</commit_message>
<xml_diff>
--- a/Model_Parameters.xlsx
+++ b/Model_Parameters.xlsx
@@ -5,15 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krishrao\Desktop\Laptop Backup\Krishna\Fall'21\IOE 574\Term Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krishrao\Desktop\Laptop Backup\Krishna\Fall'21\IOE 574\Term Project\IOE574_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7BDAEA7-548B-4816-B554-D24F217F7EA4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D075947-856E-43AB-9208-787F487EF54F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Routes" sheetId="1" r:id="rId1"/>
+    <sheet name="Demands" sheetId="2" r:id="rId2"/>
+    <sheet name="Possible_Updates" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>route_1_mean</t>
   </si>
@@ -61,6 +63,27 @@
   </si>
   <si>
     <t>route_2_std</t>
+  </si>
+  <si>
+    <t>Route</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>charge</t>
+  </si>
+  <si>
+    <t>* Updating 1st stop of bus as deployment with mean 0 and std 0</t>
   </si>
 </sst>
 </file>
@@ -96,8 +119,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,8 +404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -440,7 +464,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -449,7 +473,7 @@
         <v>0.25</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <v>1.5</v>
@@ -458,7 +482,7 @@
         <v>0.25</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2">
         <v>5</v>
@@ -467,7 +491,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K2">
         <v>5</v>
@@ -478,7 +502,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3">
         <v>12</v>
@@ -487,7 +511,7 @@
         <v>5</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <v>5</v>
@@ -496,7 +520,7 @@
         <v>2</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -505,7 +529,7 @@
         <v>0.5</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K3">
         <v>1</v>
@@ -516,7 +540,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -525,7 +549,7 @@
         <v>0.5</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -534,7 +558,7 @@
         <v>0.5</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4">
         <v>7</v>
@@ -543,7 +567,7 @@
         <v>2</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4">
         <v>7</v>
@@ -554,7 +578,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="G5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5">
         <v>0.75</v>
@@ -563,7 +587,7 @@
         <v>1.5</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5">
         <v>0.75</v>
@@ -574,7 +598,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="G6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6">
         <v>5</v>
@@ -583,7 +607,7 @@
         <v>1.5</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6">
         <v>5</v>
@@ -594,7 +618,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="G7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7">
         <v>1.2</v>
@@ -605,13 +629,128 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="G8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8">
         <v>4</v>
       </c>
       <c r="I8">
         <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6127B80-B336-49A8-B63D-818655E54FC4}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>75</v>
+      </c>
+      <c r="F2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>-180</v>
+      </c>
+      <c r="E3">
+        <v>120</v>
+      </c>
+      <c r="F3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>45</v>
+      </c>
+      <c r="F4">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD6B424-442A-444D-AE06-F335FF6D6F4D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Functional Programming Update to Main Program
</commit_message>
<xml_diff>
--- a/Model_Parameters.xlsx
+++ b/Model_Parameters.xlsx
@@ -8,26 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krishrao\Desktop\Laptop Backup\Krishna\Fall'21\IOE 574\Term Project\IOE574_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D075947-856E-43AB-9208-787F487EF54F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA715E0-B2A6-45D7-9294-6E84FC78E76D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Routes" sheetId="1" r:id="rId1"/>
     <sheet name="Demands" sheetId="2" r:id="rId2"/>
     <sheet name="Possible_Updates" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>route_1_mean</t>
   </si>
@@ -84,6 +93,45 @@
   </si>
   <si>
     <t>* Updating 1st stop of bus as deployment with mean 0 and std 0</t>
+  </si>
+  <si>
+    <t>Gallons per hour</t>
+  </si>
+  <si>
+    <t>lts per minute</t>
+  </si>
+  <si>
+    <t>Electric</t>
+  </si>
+  <si>
+    <t>Fuel Running</t>
+  </si>
+  <si>
+    <t>Fuel Idle</t>
+  </si>
+  <si>
+    <t>ReFueling</t>
+  </si>
+  <si>
+    <t>30-34</t>
+  </si>
+  <si>
+    <t>https://www.quora.com/What-is-the-flow-rate-of-gasoline-station-fuel-dispensers-in-liters-per-second</t>
+  </si>
+  <si>
+    <t>https://www.energy.gov/eere/vehicles/fact-861-february-23-2015-idle-fuel-consumption-selected-gasoline-and-diesel-vehicles</t>
+  </si>
+  <si>
+    <t>https://www.google.com/search?q=average+fuel+consumtion+of+transit+bus+per+hour&amp;rlz=1C1GCEA_enUS970US970&amp;oq=average+fuel+consumtion+of+transit+bus+per+hour&amp;aqs=chrome..69i57j33i10i22i29i30.16846j0j9&amp;sourceid=chrome&amp;ie=UTF-8</t>
+  </si>
+  <si>
+    <t>route_3_index</t>
+  </si>
+  <si>
+    <t>route_3_mean</t>
+  </si>
+  <si>
+    <t>route_3_std</t>
   </si>
 </sst>
 </file>
@@ -402,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -422,9 +470,12 @@
     <col min="10" max="10" width="12.77734375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -461,8 +512,17 @@
       <c r="L1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -499,8 +559,17 @@
       <c r="L2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>5</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0</v>
       </c>
@@ -517,7 +586,7 @@
         <v>5</v>
       </c>
       <c r="F3">
-        <v>2</v>
+        <v>0.25</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -537,8 +606,17 @@
       <c r="L3">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -575,8 +653,17 @@
       <c r="L4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>7</v>
+      </c>
+      <c r="O4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G5">
         <v>0</v>
       </c>
@@ -595,8 +682,17 @@
       <c r="L5">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0.75</v>
+      </c>
+      <c r="O5">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G6">
         <v>1</v>
       </c>
@@ -615,8 +711,17 @@
       <c r="L6">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>5</v>
+      </c>
+      <c r="O6">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G7">
         <v>0</v>
       </c>
@@ -627,7 +732,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G8">
         <v>1</v>
       </c>
@@ -648,7 +753,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -678,10 +783,10 @@
         <v>1</v>
       </c>
       <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
         <v>2</v>
-      </c>
-      <c r="C2">
-        <v>3</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -710,7 +815,7 @@
         <v>120</v>
       </c>
       <c r="F3">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -718,7 +823,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -730,7 +835,7 @@
         <v>45</v>
       </c>
       <c r="F4">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -740,17 +845,84 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD6B424-442A-444D-AE06-F335FF6D6F4D}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.77734375" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7">
+        <f>F8/60</f>
+        <v>7.161533333333335E-2</v>
+      </c>
+      <c r="E7">
+        <f>8.9/100</f>
+        <v>8.900000000000001E-2</v>
+      </c>
+      <c r="F7">
+        <v>48.28</v>
+      </c>
+      <c r="G7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8">
+        <v>0.97</v>
+      </c>
+      <c r="C8">
+        <f>3.78*B8/60</f>
+        <v>6.1109999999999998E-2</v>
+      </c>
+      <c r="F8">
+        <f>E7*F7</f>
+        <v>4.296920000000001</v>
+      </c>
+      <c r="G8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 2.5 Everything is working (hopefully!)
</commit_message>
<xml_diff>
--- a/Model_Parameters.xlsx
+++ b/Model_Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krishrao\Desktop\Laptop Backup\Krishna\Fall'21\IOE 574\Term Project\IOE574_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF96E49-95C1-4AE0-9C73-A9D40C02D1C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52226B8D-A3BC-46E2-ACAC-EB738255ADC8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demands" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="Possible_Updates" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -629,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FD1DF37-C7D6-40AA-9060-57C1756E1061}">
   <dimension ref="A1:R52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3382,7 +3381,7 @@
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>